<commit_message>
report, rules, mcha structure
</commit_message>
<xml_diff>
--- a/MCHA Team Structures.xlsx
+++ b/MCHA Team Structures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\NU-Racing-Lead-MCHA-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F33DAF-7A02-480D-97C2-4A0A8B4E6513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB640CF8-CA25-4002-B440-FDD9CB6FED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F73F5827-12D0-4F6E-B65D-146681A7A38E}"/>
   </bookViews>
@@ -204,12 +204,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -217,7 +214,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E15" sqref="E15"/>
+      <selection pane="topRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,59 +573,59 @@
     <col min="16" max="16" width="5.7109375" customWidth="1"/>
     <col min="17" max="17" width="22.140625" customWidth="1"/>
     <col min="19" max="19" width="5.7109375" customWidth="1"/>
-    <col min="20" max="20" width="24.28515625" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
     <col min="22" max="22" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>'Plan A - 17 Ppl'!B2</f>
         <v>PLAN A || People Count = 17</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="str">
+      <c r="C2" s="9"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="9" t="str">
         <f>'Plan B - 10 Ppl'!B2</f>
         <v>PLAN B || People Count = 10</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2" t="str">
+      <c r="F2" s="9"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="9" t="str">
         <f>'Plan C - 10 Ppl'!B2</f>
         <v>PLAN C || People Count = 10</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="2" t="str">
+      <c r="I2" s="9"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="9" t="str">
         <f>'Plan D - 9 Ppl'!B2</f>
         <v>PLAN D || People Count = 9</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="2" t="str">
+      <c r="L2" s="9"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="9" t="str">
         <f>'Plan E - 8 Ppl'!B2</f>
         <v>PLAN E || People Count = 8</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="2" t="str">
+      <c r="O2" s="9"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="9" t="str">
         <f>'Plan F - 7 Ppl'!B2</f>
         <v>PLAN F || People Count = 7</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="2" t="str">
+      <c r="R2" s="9"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="9" t="str">
         <f>'Plan G - 6 Ppl'!B2</f>
         <v>PLAN G || People Count = 6 (Including me)</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="3"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="2"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -640,7 +639,7 @@
         <f>'Plan A - 17 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="2"/>
       <c r="E3" t="str">
         <f>'Plan B - 10 Ppl'!B3</f>
         <v>New Person</v>
@@ -649,7 +648,7 @@
         <f>'Plan B - 10 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2"/>
       <c r="H3" t="str">
         <f>'Plan C - 10 Ppl'!B3</f>
         <v>New Person</v>
@@ -658,7 +657,7 @@
         <f>'Plan C - 10 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="2"/>
       <c r="K3" t="str">
         <f>'Plan D - 9 Ppl'!B3</f>
         <v>New Person</v>
@@ -667,7 +666,7 @@
         <f>'Plan D - 9 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="2"/>
       <c r="N3" t="str">
         <f>'Plan E - 8 Ppl'!B3</f>
         <v>New Person</v>
@@ -676,7 +675,7 @@
         <f>'Plan E - 8 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="P3" s="3"/>
+      <c r="P3" s="2"/>
       <c r="Q3" t="str">
         <f>'Plan F - 7 Ppl'!B3</f>
         <v>New Person</v>
@@ -685,7 +684,7 @@
         <f>'Plan F - 7 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="S3" s="3"/>
+      <c r="S3" s="2"/>
       <c r="T3" t="str">
         <f>'Plan G - 6 Ppl'!B3</f>
         <v>New Person</v>
@@ -694,7 +693,7 @@
         <f>'Plan G - 6 Ppl'!C3</f>
         <v>1</v>
       </c>
-      <c r="V3" s="3"/>
+      <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -708,7 +707,7 @@
         <f>'Plan A - 17 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B4</f>
         <v>New Person</v>
@@ -717,7 +716,7 @@
         <f>'Plan B - 10 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B4</f>
         <v>New Person</v>
@@ -726,7 +725,7 @@
         <f>'Plan C - 10 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B4</f>
         <v>New Person</v>
@@ -735,7 +734,7 @@
         <f>'Plan D - 9 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="M4" s="3"/>
+      <c r="M4" s="2"/>
       <c r="N4" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B4</f>
         <v>New Person</v>
@@ -744,25 +743,25 @@
         <f>'Plan E - 8 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="2"/>
       <c r="Q4" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B4</f>
         <v>New Person</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="4">
         <f>'Plan F - 7 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="S4" s="3"/>
+      <c r="S4" s="2"/>
       <c r="T4" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B4</f>
         <v>Me</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="4">
         <f>'Plan G - 6 Ppl'!C4</f>
         <v>2</v>
       </c>
-      <c r="V4" s="3"/>
+      <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -776,7 +775,7 @@
         <f>'Plan A - 17 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="2"/>
       <c r="E5" t="str">
         <f>'Plan B - 10 Ppl'!B5</f>
         <v>New Person</v>
@@ -785,7 +784,7 @@
         <f>'Plan B - 10 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
       <c r="H5" t="str">
         <f>'Plan C - 10 Ppl'!B5</f>
         <v>New Person</v>
@@ -794,7 +793,7 @@
         <f>'Plan C - 10 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="2"/>
       <c r="K5" t="str">
         <f>'Plan D - 9 Ppl'!B5</f>
         <v>New Person</v>
@@ -803,34 +802,34 @@
         <f>'Plan D - 9 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="M5" s="3"/>
+      <c r="M5" s="2"/>
       <c r="N5" t="str">
         <f>'Plan E - 8 Ppl'!B5</f>
         <v>New Person</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5">
         <f>'Plan E - 8 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="2"/>
       <c r="Q5" t="str">
         <f>'Plan F - 7 Ppl'!B5</f>
         <v>New Person</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5">
         <f>'Plan F - 7 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="S5" s="3"/>
+      <c r="S5" s="2"/>
       <c r="T5" t="str">
         <f>'Plan G - 6 Ppl'!B5</f>
         <v>New Person</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <f>'Plan G - 6 Ppl'!C5</f>
         <v>3</v>
       </c>
-      <c r="V5" s="3"/>
+      <c r="V5" s="2"/>
     </row>
     <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -844,7 +843,7 @@
         <f>'Plan A - 17 Ppl'!C6</f>
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B6</f>
         <v>New Person</v>
@@ -853,7 +852,7 @@
         <f>'Plan B - 10 Ppl'!C6</f>
         <v>4</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B6</f>
         <v>New Person</v>
@@ -862,7 +861,7 @@
         <f>'Plan C - 10 Ppl'!C6</f>
         <v>4</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B6</f>
         <v>New Person</v>
@@ -871,7 +870,7 @@
         <f>'Plan D - 9 Ppl'!C6</f>
         <v>4</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B6</f>
         <v>New Person</v>
@@ -880,7 +879,7 @@
         <f>'Plan E - 8 Ppl'!C6</f>
         <v>4</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="2"/>
       <c r="Q6" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B6</f>
         <v>New Person</v>
@@ -889,16 +888,16 @@
         <f>'Plan F - 7 Ppl'!C6</f>
         <v>4</v>
       </c>
-      <c r="S6" s="3"/>
+      <c r="S6" s="2"/>
       <c r="T6" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B6</f>
         <v>New Person</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="5">
         <f>'Plan G - 6 Ppl'!C6</f>
         <v>3</v>
       </c>
-      <c r="V6" s="3"/>
+      <c r="V6" s="2"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -912,7 +911,7 @@
         <f>'Plan A - 17 Ppl'!C7</f>
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="2"/>
       <c r="E7" t="str">
         <f>'Plan B - 10 Ppl'!B7</f>
         <v>New Person</v>
@@ -921,7 +920,7 @@
         <f>'Plan B - 10 Ppl'!C7</f>
         <v>5</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="2"/>
       <c r="H7" t="str">
         <f>'Plan C - 10 Ppl'!B7</f>
         <v>ENGG3200</v>
@@ -930,7 +929,7 @@
         <f>'Plan C - 10 Ppl'!C7</f>
         <v>5</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="2"/>
       <c r="K7" t="str">
         <f>'Plan D - 9 Ppl'!B7</f>
         <v>New Person</v>
@@ -939,7 +938,7 @@
         <f>'Plan D - 9 Ppl'!C7</f>
         <v>5</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="2"/>
       <c r="N7" t="str">
         <f>'Plan E - 8 Ppl'!B7</f>
         <v>New Person</v>
@@ -948,7 +947,7 @@
         <f>'Plan E - 8 Ppl'!C7</f>
         <v>5</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="2"/>
       <c r="Q7" t="str">
         <f>'Plan F - 7 Ppl'!B7</f>
         <v>ENGG3200</v>
@@ -957,7 +956,7 @@
         <f>'Plan F - 7 Ppl'!C7</f>
         <v>5</v>
       </c>
-      <c r="S7" s="3"/>
+      <c r="S7" s="2"/>
       <c r="T7" t="str">
         <f>'Plan G - 6 Ppl'!B7</f>
         <v>ENGG3200</v>
@@ -966,7 +965,7 @@
         <f>'Plan G - 6 Ppl'!C7</f>
         <v>4</v>
       </c>
-      <c r="V7" s="3"/>
+      <c r="V7" s="2"/>
     </row>
     <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -980,7 +979,7 @@
         <f>'Plan A - 17 Ppl'!C8</f>
         <v>6</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B8</f>
         <v>New Person</v>
@@ -989,7 +988,7 @@
         <f>'Plan B - 10 Ppl'!C8</f>
         <v>6</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B8</f>
         <v>New Person</v>
@@ -998,7 +997,7 @@
         <f>'Plan C - 10 Ppl'!C8</f>
         <v>6</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B8</f>
         <v>New Person</v>
@@ -1007,34 +1006,34 @@
         <f>'Plan D - 9 Ppl'!C8</f>
         <v>6</v>
       </c>
-      <c r="M8" s="3"/>
+      <c r="M8" s="2"/>
       <c r="N8" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B8</f>
         <v>New Person</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="6">
         <f>'Plan E - 8 Ppl'!C8</f>
         <v>6</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="2"/>
       <c r="Q8" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B8</f>
         <v>New Person</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
         <f>'Plan F - 7 Ppl'!C8</f>
         <v>6</v>
       </c>
-      <c r="S8" s="3"/>
+      <c r="S8" s="2"/>
       <c r="T8" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B8</f>
         <v>New Person</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8" s="6">
         <f>'Plan G - 6 Ppl'!C8</f>
         <v>5</v>
       </c>
-      <c r="V8" s="3"/>
+      <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1048,7 +1047,7 @@
         <f>'Plan A - 17 Ppl'!C9</f>
         <v>7</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="2"/>
       <c r="E9" t="str">
         <f>'Plan B - 10 Ppl'!B9</f>
         <v>New Person</v>
@@ -1057,7 +1056,7 @@
         <f>'Plan B - 10 Ppl'!C9</f>
         <v>7</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="2"/>
       <c r="H9" t="str">
         <f>'Plan C - 10 Ppl'!B9</f>
         <v>New Person</v>
@@ -1066,7 +1065,7 @@
         <f>'Plan C - 10 Ppl'!C9</f>
         <v>7</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="2"/>
       <c r="K9" t="str">
         <f>'Plan D - 9 Ppl'!B9</f>
         <v>New Person</v>
@@ -1075,34 +1074,34 @@
         <f>'Plan D - 9 Ppl'!C9</f>
         <v>7</v>
       </c>
-      <c r="M9" s="3"/>
+      <c r="M9" s="2"/>
       <c r="N9" t="str">
         <f>'Plan E - 8 Ppl'!B9</f>
         <v>New Person</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="6">
         <f>'Plan E - 8 Ppl'!C9</f>
         <v>6</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="2"/>
       <c r="Q9" t="str">
         <f>'Plan F - 7 Ppl'!B9</f>
         <v>New Person</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="6">
         <f>'Plan F - 7 Ppl'!C9</f>
         <v>6</v>
       </c>
-      <c r="S9" s="3"/>
+      <c r="S9" s="2"/>
       <c r="T9" t="str">
         <f>'Plan G - 6 Ppl'!B9</f>
         <v>New Person</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9" s="6">
         <f>'Plan G - 6 Ppl'!C9</f>
         <v>5</v>
       </c>
-      <c r="V9" s="3"/>
+      <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1116,7 +1115,7 @@
         <f>'Plan A - 17 Ppl'!C10</f>
         <v>8</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B10</f>
         <v>New Person</v>
@@ -1125,7 +1124,7 @@
         <f>'Plan B - 10 Ppl'!C10</f>
         <v>8</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B10</f>
         <v>New Person</v>
@@ -1134,7 +1133,7 @@
         <f>'Plan C - 10 Ppl'!C10</f>
         <v>8</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B10</f>
         <v>New Person</v>
@@ -1143,7 +1142,7 @@
         <f>'Plan D - 9 Ppl'!C10</f>
         <v>8</v>
       </c>
-      <c r="M10" s="3"/>
+      <c r="M10" s="2"/>
       <c r="N10" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B10</f>
         <v>New Person</v>
@@ -1152,7 +1151,7 @@
         <f>'Plan E - 8 Ppl'!C10</f>
         <v>7</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="P10" s="2"/>
       <c r="Q10" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B10</f>
         <v>New Person</v>
@@ -1161,7 +1160,7 @@
         <f>'Plan F - 7 Ppl'!C10</f>
         <v>7</v>
       </c>
-      <c r="S10" s="3"/>
+      <c r="S10" s="2"/>
       <c r="T10" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B10</f>
         <v>New Person</v>
@@ -1170,7 +1169,7 @@
         <f>'Plan G - 6 Ppl'!C10</f>
         <v>6</v>
       </c>
-      <c r="V10" s="3"/>
+      <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1184,7 +1183,7 @@
         <f>'Plan A - 17 Ppl'!C11</f>
         <v>9</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="2"/>
       <c r="E11" t="str">
         <f>'Plan B - 10 Ppl'!B11</f>
         <v>New Person - Junior</v>
@@ -1193,7 +1192,7 @@
         <f>'Plan B - 10 Ppl'!C11</f>
         <v>9</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="2"/>
       <c r="H11" t="str">
         <f>'Plan C - 10 Ppl'!B11</f>
         <v>New Person - Junior</v>
@@ -1202,7 +1201,7 @@
         <f>'Plan C - 10 Ppl'!C11</f>
         <v>9</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="2"/>
       <c r="K11" t="str">
         <f>'Plan D - 9 Ppl'!B11</f>
         <v>New Person - Junior</v>
@@ -1211,7 +1210,7 @@
         <f>'Plan D - 9 Ppl'!C11</f>
         <v>9</v>
       </c>
-      <c r="M11" s="3"/>
+      <c r="M11" s="2"/>
       <c r="N11" t="str">
         <f>'Plan E - 8 Ppl'!B11</f>
         <v>New Person - Junior</v>
@@ -1220,25 +1219,25 @@
         <f>'Plan E - 8 Ppl'!C11</f>
         <v>8</v>
       </c>
-      <c r="P11" s="3"/>
+      <c r="P11" s="2"/>
       <c r="Q11" t="str">
         <f>'Plan F - 7 Ppl'!B11</f>
         <v>New Person</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="4">
         <f>'Plan F - 7 Ppl'!C11</f>
         <v>2</v>
       </c>
-      <c r="S11" s="3"/>
+      <c r="S11" s="2"/>
       <c r="T11" t="str">
         <f>'Plan G - 6 Ppl'!B11</f>
         <v>Me</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="4">
         <f>'Plan G - 6 Ppl'!C11</f>
         <v>2</v>
       </c>
-      <c r="V11" s="3"/>
+      <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1252,7 +1251,7 @@
         <f>'Plan A - 17 Ppl'!C12</f>
         <v>10</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B12</f>
         <v>New Person</v>
@@ -1261,7 +1260,7 @@
         <f>'Plan B - 10 Ppl'!C12</f>
         <v>10</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B12</f>
         <v>New Person</v>
@@ -1270,23 +1269,23 @@
         <f>'Plan C - 10 Ppl'!C12</f>
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="V12" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="V13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1300,13 +1299,13 @@
         <f>'Plan A - 17 Ppl'!C14</f>
         <v>11</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="V14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1320,13 +1319,13 @@
         <f>'Plan A - 17 Ppl'!C15</f>
         <v>12</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="V15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1340,13 +1339,13 @@
         <f>'Plan A - 17 Ppl'!C16</f>
         <v>13</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="V16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1360,13 +1359,13 @@
         <f>'Plan A - 17 Ppl'!C17</f>
         <v>14</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="V17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1380,13 +1379,13 @@
         <f>'Plan A - 17 Ppl'!C18</f>
         <v>15</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="V18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1400,13 +1399,13 @@
         <f>'Plan A - 17 Ppl'!C19</f>
         <v>16</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="V19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="V19" s="2"/>
     </row>
     <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1420,63 +1419,63 @@
         <f>'Plan A - 17 Ppl'!C20</f>
         <v>17</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="V20" s="3"/>
-    </row>
-    <row r="22" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="D20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="22" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>'Plan A - 17 Ppl'!B23</f>
         <v>PLAN A || People Count = 17</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="2" t="str">
+      <c r="C23" s="9"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="9" t="str">
         <f>'Plan B - 10 Ppl'!B23</f>
         <v>PLAN B || People Count = 10</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="2" t="str">
+      <c r="F23" s="9"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="9" t="str">
         <f>'Plan C - 10 Ppl'!B23</f>
         <v>PLAN C || People Count = 10</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="2" t="str">
+      <c r="I23" s="9"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="9" t="str">
         <f>'Plan D - 9 Ppl'!B23</f>
         <v>PLAN D || People Count = 9</v>
       </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="2" t="str">
+      <c r="L23" s="9"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="9" t="str">
         <f>'Plan E - 8 Ppl'!B23</f>
         <v>PLAN E || People Count = 8</v>
       </c>
-      <c r="O23" s="2"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="2" t="str">
+      <c r="O23" s="9"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="9" t="str">
         <f>'Plan F - 7 Ppl'!B23</f>
         <v>PLAN F || People Count = 7</v>
       </c>
-      <c r="R23" s="2"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="2" t="str">
+      <c r="R23" s="9"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="9" t="str">
         <f>'Plan G - 6 Ppl'!B23</f>
         <v>PLAN G || People Count = 6 (Including me)</v>
       </c>
-      <c r="U23" s="2"/>
-      <c r="V23" s="3"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1490,7 +1489,7 @@
         <f>'Plan A - 17 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="2"/>
       <c r="E24" t="str">
         <f>'Plan B - 10 Ppl'!B24</f>
         <v>Hayward</v>
@@ -1499,7 +1498,7 @@
         <f>'Plan B - 10 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="2"/>
       <c r="H24" t="str">
         <f>'Plan C - 10 Ppl'!B24</f>
         <v>Hayward</v>
@@ -1508,7 +1507,7 @@
         <f>'Plan C - 10 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="J24" s="3"/>
+      <c r="J24" s="2"/>
       <c r="K24" t="str">
         <f>'Plan D - 9 Ppl'!B24</f>
         <v>Hayward</v>
@@ -1517,7 +1516,7 @@
         <f>'Plan D - 9 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="M24" s="3"/>
+      <c r="M24" s="2"/>
       <c r="N24" t="str">
         <f>'Plan E - 8 Ppl'!B24</f>
         <v>Hayward</v>
@@ -1526,7 +1525,7 @@
         <f>'Plan E - 8 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="P24" s="3"/>
+      <c r="P24" s="2"/>
       <c r="Q24" t="str">
         <f>'Plan F - 7 Ppl'!B24</f>
         <v>Hayward</v>
@@ -1535,7 +1534,7 @@
         <f>'Plan F - 7 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="S24" s="3"/>
+      <c r="S24" s="2"/>
       <c r="T24" t="str">
         <f>'Plan G - 6 Ppl'!B24</f>
         <v>Hayward</v>
@@ -1544,7 +1543,7 @@
         <f>'Plan G - 6 Ppl'!C24</f>
         <v>1</v>
       </c>
-      <c r="V24" s="3"/>
+      <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1558,7 +1557,7 @@
         <f>'Plan A - 17 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B25</f>
         <v>New Person</v>
@@ -1567,7 +1566,7 @@
         <f>'Plan B - 10 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B25</f>
         <v>New Person</v>
@@ -1576,7 +1575,7 @@
         <f>'Plan C - 10 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="J25" s="3"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B25</f>
         <v>New Person</v>
@@ -1585,7 +1584,7 @@
         <f>'Plan D - 9 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="M25" s="3"/>
+      <c r="M25" s="2"/>
       <c r="N25" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B25</f>
         <v>New Person</v>
@@ -1594,25 +1593,25 @@
         <f>'Plan E - 8 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="P25" s="3"/>
+      <c r="P25" s="2"/>
       <c r="Q25" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B25</f>
         <v>New Person</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25" s="4">
         <f>'Plan F - 7 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="S25" s="3"/>
+      <c r="S25" s="2"/>
       <c r="T25" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B25</f>
         <v>Me</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="4">
         <f>'Plan G - 6 Ppl'!C25</f>
         <v>2</v>
       </c>
-      <c r="V25" s="3"/>
+      <c r="V25" s="2"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1626,7 +1625,7 @@
         <f>'Plan A - 17 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="2"/>
       <c r="E26" t="str">
         <f>'Plan B - 10 Ppl'!B26</f>
         <v>New Person</v>
@@ -1635,7 +1634,7 @@
         <f>'Plan B - 10 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="2"/>
       <c r="H26" t="str">
         <f>'Plan C - 10 Ppl'!B26</f>
         <v>New Person</v>
@@ -1644,7 +1643,7 @@
         <f>'Plan C - 10 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="J26" s="3"/>
+      <c r="J26" s="2"/>
       <c r="K26" t="str">
         <f>'Plan D - 9 Ppl'!B26</f>
         <v>New Person</v>
@@ -1653,34 +1652,34 @@
         <f>'Plan D - 9 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="M26" s="3"/>
+      <c r="M26" s="2"/>
       <c r="N26" t="str">
         <f>'Plan E - 8 Ppl'!B26</f>
         <v>New Person</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26">
         <f>'Plan E - 8 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="P26" s="2"/>
       <c r="Q26" t="str">
         <f>'Plan F - 7 Ppl'!B26</f>
         <v>New Person</v>
       </c>
-      <c r="R26" s="10">
+      <c r="R26">
         <f>'Plan F - 7 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="S26" s="3"/>
+      <c r="S26" s="2"/>
       <c r="T26" t="str">
         <f>'Plan G - 6 Ppl'!B26</f>
         <v>New Person</v>
       </c>
-      <c r="U26" s="6">
+      <c r="U26" s="5">
         <f>'Plan G - 6 Ppl'!C26</f>
         <v>3</v>
       </c>
-      <c r="V26" s="3"/>
+      <c r="V26" s="2"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1694,7 +1693,7 @@
         <f>'Plan A - 17 Ppl'!C27</f>
         <v>4</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B27</f>
         <v>New Person</v>
@@ -1703,7 +1702,7 @@
         <f>'Plan B - 10 Ppl'!C27</f>
         <v>4</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="2"/>
       <c r="H27" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B27</f>
         <v>New Person</v>
@@ -1712,7 +1711,7 @@
         <f>'Plan C - 10 Ppl'!C27</f>
         <v>4</v>
       </c>
-      <c r="J27" s="3"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B27</f>
         <v>New Person</v>
@@ -1721,7 +1720,7 @@
         <f>'Plan D - 9 Ppl'!C27</f>
         <v>4</v>
       </c>
-      <c r="M27" s="3"/>
+      <c r="M27" s="2"/>
       <c r="N27" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B27</f>
         <v>New Person</v>
@@ -1730,7 +1729,7 @@
         <f>'Plan E - 8 Ppl'!C27</f>
         <v>4</v>
       </c>
-      <c r="P27" s="3"/>
+      <c r="P27" s="2"/>
       <c r="Q27" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B27</f>
         <v>New Person</v>
@@ -1739,16 +1738,16 @@
         <f>'Plan F - 7 Ppl'!C27</f>
         <v>4</v>
       </c>
-      <c r="S27" s="3"/>
+      <c r="S27" s="2"/>
       <c r="T27" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B27</f>
         <v>New Person</v>
       </c>
-      <c r="U27" s="6">
+      <c r="U27" s="5">
         <f>'Plan G - 6 Ppl'!C27</f>
         <v>3</v>
       </c>
-      <c r="V27" s="3"/>
+      <c r="V27" s="2"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1762,7 +1761,7 @@
         <f>'Plan A - 17 Ppl'!C28</f>
         <v>5</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="2"/>
       <c r="E28" t="str">
         <f>'Plan B - 10 Ppl'!B28</f>
         <v>New Person</v>
@@ -1771,7 +1770,7 @@
         <f>'Plan B - 10 Ppl'!C28</f>
         <v>5</v>
       </c>
-      <c r="G28" s="3"/>
+      <c r="G28" s="2"/>
       <c r="H28" t="str">
         <f>'Plan C - 10 Ppl'!B28</f>
         <v>ENGG3200</v>
@@ -1780,7 +1779,7 @@
         <f>'Plan C - 10 Ppl'!C28</f>
         <v>5</v>
       </c>
-      <c r="J28" s="3"/>
+      <c r="J28" s="2"/>
       <c r="K28" t="str">
         <f>'Plan D - 9 Ppl'!B28</f>
         <v>New Person</v>
@@ -1789,7 +1788,7 @@
         <f>'Plan D - 9 Ppl'!C28</f>
         <v>5</v>
       </c>
-      <c r="M28" s="3"/>
+      <c r="M28" s="2"/>
       <c r="N28" t="str">
         <f>'Plan E - 8 Ppl'!B28</f>
         <v>New Person</v>
@@ -1798,7 +1797,7 @@
         <f>'Plan E - 8 Ppl'!C28</f>
         <v>5</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="2"/>
       <c r="Q28" t="str">
         <f>'Plan F - 7 Ppl'!B28</f>
         <v>New Person</v>
@@ -1807,7 +1806,7 @@
         <f>'Plan F - 7 Ppl'!C28</f>
         <v>5</v>
       </c>
-      <c r="S28" s="3"/>
+      <c r="S28" s="2"/>
       <c r="T28" t="str">
         <f>'Plan G - 6 Ppl'!B28</f>
         <v>ENGG3200</v>
@@ -1816,7 +1815,7 @@
         <f>'Plan G - 6 Ppl'!C28</f>
         <v>4</v>
       </c>
-      <c r="V28" s="3"/>
+      <c r="V28" s="2"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1830,7 +1829,7 @@
         <f>'Plan A - 17 Ppl'!C29</f>
         <v>6</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B29</f>
         <v>New Person</v>
@@ -1839,7 +1838,7 @@
         <f>'Plan B - 10 Ppl'!C29</f>
         <v>6</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B29</f>
         <v>New Person</v>
@@ -1848,7 +1847,7 @@
         <f>'Plan C - 10 Ppl'!C29</f>
         <v>6</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B29</f>
         <v>New Person</v>
@@ -1857,34 +1856,34 @@
         <f>'Plan D - 9 Ppl'!C29</f>
         <v>6</v>
       </c>
-      <c r="M29" s="3"/>
+      <c r="M29" s="2"/>
       <c r="N29" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B29</f>
         <v>New Person</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="6">
         <f>'Plan E - 8 Ppl'!C29</f>
         <v>6</v>
       </c>
-      <c r="P29" s="3"/>
+      <c r="P29" s="2"/>
       <c r="Q29" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B29</f>
         <v>New Person</v>
       </c>
-      <c r="R29" s="7">
+      <c r="R29" s="6">
         <f>'Plan F - 7 Ppl'!C29</f>
         <v>6</v>
       </c>
-      <c r="S29" s="3"/>
+      <c r="S29" s="2"/>
       <c r="T29" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B29</f>
         <v>New Person</v>
       </c>
-      <c r="U29" s="7">
+      <c r="U29" s="6">
         <f>'Plan G - 6 Ppl'!C29</f>
         <v>5</v>
       </c>
-      <c r="V29" s="3"/>
+      <c r="V29" s="2"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1898,7 +1897,7 @@
         <f>'Plan A - 17 Ppl'!C30</f>
         <v>7</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="2"/>
       <c r="E30" t="str">
         <f>'Plan B - 10 Ppl'!B30</f>
         <v>New Person</v>
@@ -1907,7 +1906,7 @@
         <f>'Plan B - 10 Ppl'!C30</f>
         <v>7</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="2"/>
       <c r="H30" t="str">
         <f>'Plan C - 10 Ppl'!B30</f>
         <v>New Person</v>
@@ -1916,7 +1915,7 @@
         <f>'Plan C - 10 Ppl'!C30</f>
         <v>7</v>
       </c>
-      <c r="J30" s="3"/>
+      <c r="J30" s="2"/>
       <c r="K30" t="str">
         <f>'Plan D - 9 Ppl'!B30</f>
         <v>New Person</v>
@@ -1925,34 +1924,34 @@
         <f>'Plan D - 9 Ppl'!C30</f>
         <v>7</v>
       </c>
-      <c r="M30" s="3"/>
+      <c r="M30" s="2"/>
       <c r="N30" t="str">
         <f>'Plan E - 8 Ppl'!B30</f>
         <v>New Person</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="6">
         <f>'Plan E - 8 Ppl'!C30</f>
         <v>6</v>
       </c>
-      <c r="P30" s="3"/>
+      <c r="P30" s="2"/>
       <c r="Q30" t="str">
         <f>'Plan F - 7 Ppl'!B30</f>
         <v>New Person</v>
       </c>
-      <c r="R30" s="7">
+      <c r="R30" s="6">
         <f>'Plan F - 7 Ppl'!C30</f>
         <v>6</v>
       </c>
-      <c r="S30" s="3"/>
+      <c r="S30" s="2"/>
       <c r="T30" t="str">
         <f>'Plan G - 6 Ppl'!B30</f>
         <v>New Person</v>
       </c>
-      <c r="U30" s="7">
+      <c r="U30" s="6">
         <f>'Plan G - 6 Ppl'!C30</f>
         <v>5</v>
       </c>
-      <c r="V30" s="3"/>
+      <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1966,7 +1965,7 @@
         <f>'Plan A - 17 Ppl'!C31</f>
         <v>8</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B31</f>
         <v>New Person</v>
@@ -1975,7 +1974,7 @@
         <f>'Plan B - 10 Ppl'!C31</f>
         <v>8</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B31</f>
         <v>New Person</v>
@@ -1984,7 +1983,7 @@
         <f>'Plan C - 10 Ppl'!C31</f>
         <v>8</v>
       </c>
-      <c r="J31" s="3"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="1" t="str">
         <f>'Plan D - 9 Ppl'!B31</f>
         <v>New Person</v>
@@ -1993,7 +1992,7 @@
         <f>'Plan D - 9 Ppl'!C31</f>
         <v>8</v>
       </c>
-      <c r="M31" s="3"/>
+      <c r="M31" s="2"/>
       <c r="N31" s="1" t="str">
         <f>'Plan E - 8 Ppl'!B31</f>
         <v>New Person</v>
@@ -2002,7 +2001,7 @@
         <f>'Plan E - 8 Ppl'!C31</f>
         <v>7</v>
       </c>
-      <c r="P31" s="3"/>
+      <c r="P31" s="2"/>
       <c r="Q31" s="1" t="str">
         <f>'Plan F - 7 Ppl'!B31</f>
         <v>New Person</v>
@@ -2011,7 +2010,7 @@
         <f>'Plan F - 7 Ppl'!C31</f>
         <v>7</v>
       </c>
-      <c r="S31" s="3"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="1" t="str">
         <f>'Plan G - 6 Ppl'!B31</f>
         <v>New Person</v>
@@ -2020,7 +2019,7 @@
         <f>'Plan G - 6 Ppl'!C31</f>
         <v>6</v>
       </c>
-      <c r="V31" s="3"/>
+      <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2034,7 +2033,7 @@
         <f>'Plan A - 17 Ppl'!C32</f>
         <v>9</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="2"/>
       <c r="E32" t="str">
         <f>'Plan B - 10 Ppl'!B32</f>
         <v>New Person - Junior</v>
@@ -2043,7 +2042,7 @@
         <f>'Plan B - 10 Ppl'!C32</f>
         <v>9</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="2"/>
       <c r="H32" t="str">
         <f>'Plan C - 10 Ppl'!B32</f>
         <v>New Person - Junior</v>
@@ -2052,7 +2051,7 @@
         <f>'Plan C - 10 Ppl'!C32</f>
         <v>9</v>
       </c>
-      <c r="J32" s="3"/>
+      <c r="J32" s="2"/>
       <c r="K32" t="str">
         <f>'Plan D - 9 Ppl'!B32</f>
         <v>New Person - Junior</v>
@@ -2061,7 +2060,7 @@
         <f>'Plan D - 9 Ppl'!C32</f>
         <v>9</v>
       </c>
-      <c r="M32" s="3"/>
+      <c r="M32" s="2"/>
       <c r="N32" t="str">
         <f>'Plan E - 8 Ppl'!B32</f>
         <v>New Person - Junior</v>
@@ -2070,25 +2069,25 @@
         <f>'Plan E - 8 Ppl'!C32</f>
         <v>8</v>
       </c>
-      <c r="P32" s="3"/>
+      <c r="P32" s="2"/>
       <c r="Q32" t="str">
         <f>'Plan F - 7 Ppl'!B32</f>
         <v>New Person</v>
       </c>
-      <c r="R32" s="5">
+      <c r="R32" s="4">
         <f>'Plan F - 7 Ppl'!C32</f>
         <v>2</v>
       </c>
-      <c r="S32" s="3"/>
+      <c r="S32" s="2"/>
       <c r="T32" t="str">
         <f>'Plan G - 6 Ppl'!B32</f>
         <v>Me</v>
       </c>
-      <c r="U32" s="5">
+      <c r="U32" s="4">
         <f>'Plan G - 6 Ppl'!C32</f>
         <v>2</v>
       </c>
-      <c r="V32" s="3"/>
+      <c r="V32" s="2"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -2102,7 +2101,7 @@
         <f>'Plan A - 17 Ppl'!C33</f>
         <v>10</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="1" t="str">
         <f>'Plan B - 10 Ppl'!B33</f>
         <v>New Person</v>
@@ -2111,7 +2110,7 @@
         <f>'Plan B - 10 Ppl'!C33</f>
         <v>10</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="2"/>
       <c r="H33" s="1" t="str">
         <f>'Plan C - 10 Ppl'!B33</f>
         <v>New Person</v>
@@ -2120,31 +2119,31 @@
         <f>'Plan C - 10 Ppl'!C33</f>
         <v>10</v>
       </c>
-      <c r="J33" s="3"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="3"/>
+      <c r="M33" s="2"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="3"/>
+      <c r="P33" s="2"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
-      <c r="S33" s="3"/>
+      <c r="S33" s="2"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
-      <c r="V33" s="3"/>
+      <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="V34" s="3"/>
+      <c r="D34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="V34" s="2"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -2158,25 +2157,25 @@
         <f>'Plan A - 17 Ppl'!C35</f>
         <v>11</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="2"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="2"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="3"/>
+      <c r="M35" s="2"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="3"/>
+      <c r="P35" s="2"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" s="3"/>
+      <c r="S35" s="2"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
-      <c r="V35" s="3"/>
+      <c r="V35" s="2"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2190,13 +2189,13 @@
         <f>'Plan A - 17 Ppl'!C36</f>
         <v>12</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="V36" s="3"/>
+      <c r="D36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -2210,25 +2209,25 @@
         <f>'Plan A - 17 Ppl'!C37</f>
         <v>13</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="3"/>
+      <c r="G37" s="2"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="2"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="3"/>
+      <c r="M37" s="2"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="3"/>
+      <c r="P37" s="2"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="3"/>
+      <c r="S37" s="2"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
-      <c r="V37" s="3"/>
+      <c r="V37" s="2"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2242,13 +2241,13 @@
         <f>'Plan A - 17 Ppl'!C38</f>
         <v>14</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="V38" s="3"/>
+      <c r="D38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="V38" s="2"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -2262,25 +2261,25 @@
         <f>'Plan A - 17 Ppl'!C39</f>
         <v>15</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="2"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-      <c r="M39" s="3"/>
+      <c r="M39" s="2"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="3"/>
+      <c r="P39" s="2"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="3"/>
+      <c r="S39" s="2"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
-      <c r="V39" s="3"/>
+      <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -2294,13 +2293,13 @@
         <f>'Plan A - 17 Ppl'!C40</f>
         <v>16</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="V40" s="3"/>
+      <c r="D40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="V40" s="2"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -2314,25 +2313,25 @@
         <f>'Plan A - 17 Ppl'!C41</f>
         <v>17</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="3"/>
+      <c r="G41" s="2"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="2"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="3"/>
+      <c r="M41" s="2"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="3"/>
+      <c r="P41" s="2"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="3"/>
+      <c r="S41" s="2"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-      <c r="V41" s="3"/>
+      <c r="V41" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2371,19 +2370,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN A || People Count = " &amp; C20</f>
         <v>PLAN A || People Count = 17</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2594,18 +2593,18 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN A || People Count = " &amp; C41</f>
         <v>PLAN A || People Count = 17</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2839,19 +2838,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN B || People Count = " &amp; C12</f>
         <v>PLAN B || People Count = 10</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2896,7 +2895,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C12" si="0">C5+1</f>
+        <f t="shared" ref="C6:C11" si="0">C5+1</f>
         <v>4</v>
       </c>
     </row>
@@ -3021,19 +3020,19 @@
       <c r="C20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN B || People Count = " &amp; C33</f>
         <v>PLAN B || People Count = 10</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -3226,19 +3225,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN C || People Count = " &amp; C12</f>
         <v>PLAN C || People Count = 10</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3408,19 +3407,19 @@
       <c r="C20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN C || People Count = " &amp; C33</f>
         <v>PLAN C || People Count = 10</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -3613,19 +3612,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN D || People Count = " &amp; C11</f>
         <v>PLAN D || People Count = 9</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3790,19 +3789,19 @@
       <c r="C20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN D || People Count = " &amp; C32</f>
         <v>PLAN D || People Count = 9</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -3990,19 +3989,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN E || People Count = " &amp; C11</f>
         <v>PLAN E || People Count = 8</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4068,7 +4067,7 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -4080,7 +4079,7 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>6</v>
       </c>
     </row>
@@ -4164,19 +4163,19 @@
       <c r="C20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN E || People Count = " &amp; C32</f>
         <v>PLAN E || People Count = 8</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4231,7 +4230,7 @@
         <v>17</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:C32" si="1">C27+1</f>
+        <f t="shared" ref="C28:C29" si="1">C27+1</f>
         <v>5</v>
       </c>
     </row>
@@ -4242,7 +4241,7 @@
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -4254,7 +4253,7 @@
       <c r="B30" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>6</v>
       </c>
     </row>
@@ -4266,7 +4265,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:C35" si="2">C30+1</f>
+        <f t="shared" ref="C31:C32" si="2">C30+1</f>
         <v>7</v>
       </c>
     </row>
@@ -4361,19 +4360,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN F || People Count = " &amp; 7</f>
         <v>PLAN F || People Count = 7</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4393,7 +4392,7 @@
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <f>C3+1</f>
         <v>2</v>
       </c>
@@ -4439,7 +4438,7 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -4451,7 +4450,7 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>6</v>
       </c>
     </row>
@@ -4474,7 +4473,7 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>2</v>
       </c>
     </row>
@@ -4534,19 +4533,19 @@
       <c r="C20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN F || People Count = " &amp; 7</f>
         <v>PLAN F || People Count = 7</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4566,7 +4565,7 @@
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <f>C24+1</f>
         <v>2</v>
       </c>
@@ -4601,7 +4600,7 @@
         <v>17</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:C31" si="1">C27+1</f>
+        <f t="shared" ref="C28:C29" si="1">C27+1</f>
         <v>5</v>
       </c>
     </row>
@@ -4612,7 +4611,7 @@
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -4624,7 +4623,7 @@
       <c r="B30" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>6</v>
       </c>
     </row>
@@ -4636,7 +4635,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:C34" si="2">C30+1</f>
+        <f t="shared" ref="C31" si="2">C30+1</f>
         <v>7</v>
       </c>
     </row>
@@ -4647,7 +4646,7 @@
       <c r="B32" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>2</v>
       </c>
     </row>
@@ -4730,19 +4729,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="9" t="str">
         <f>"PLAN G || People Count = " &amp; 6 &amp; " (Including me)"</f>
         <v>PLAN G || People Count = 6 (Including me)</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4762,7 +4761,7 @@
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <f>C3+1</f>
         <v>2</v>
       </c>
@@ -4774,7 +4773,7 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>3</v>
       </c>
     </row>
@@ -4785,7 +4784,7 @@
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>3</v>
       </c>
     </row>
@@ -4808,7 +4807,7 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -4820,7 +4819,7 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>5</v>
       </c>
     </row>
@@ -4843,7 +4842,7 @@
       <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>2</v>
       </c>
     </row>
@@ -4903,19 +4902,19 @@
       <c r="C20" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="9" t="str">
         <f>"PLAN G || People Count = " &amp; 6 &amp; " (Including me)"</f>
         <v>PLAN G || People Count = 6 (Including me)</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -4935,7 +4934,7 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <f>C24+1</f>
         <v>2</v>
       </c>
@@ -4947,7 +4946,7 @@
       <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>3</v>
       </c>
     </row>
@@ -4958,7 +4957,7 @@
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>3</v>
       </c>
     </row>
@@ -4970,7 +4969,7 @@
         <v>22</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:C31" si="1">C27+1</f>
+        <f t="shared" ref="C28:C29" si="1">C27+1</f>
         <v>4</v>
       </c>
     </row>
@@ -4981,7 +4980,7 @@
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -4993,7 +4992,7 @@
       <c r="B30" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>5</v>
       </c>
     </row>
@@ -5005,7 +5004,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:C34" si="2">C30+1</f>
+        <f t="shared" ref="C31" si="2">C30+1</f>
         <v>6</v>
       </c>
     </row>
@@ -5016,7 +5015,7 @@
       <c r="B32" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hv connectors, nu25 connector pinout schematic
ordered the hv connectors into files for where they will go

continued work on the nu25 schematic
</commit_message>
<xml_diff>
--- a/MCHA Team Structures.xlsx
+++ b/MCHA Team Structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\NU-Racing-Lead-MCHA-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\NU Teams\2025 Lead MCHA Github\NU-Racing-Lead-MCHA-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB640CF8-CA25-4002-B440-FDD9CB6FED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774F544-CDBC-4C56-8F9E-024F466F33AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F73F5827-12D0-4F6E-B65D-146681A7A38E}"/>
+    <workbookView xWindow="-28920" yWindow="-16440" windowWidth="29040" windowHeight="15720" xr2:uid="{F73F5827-12D0-4F6E-B65D-146681A7A38E}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="27">
   <si>
     <t>PEN</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>WITH HAYWARD</t>
+  </si>
+  <si>
+    <t>AV.One</t>
   </si>
 </sst>
 </file>
@@ -555,35 +558,35 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N19" sqref="N19"/>
+      <selection pane="topRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" customWidth="1"/>
+    <col min="17" max="17" width="22.109375" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" customWidth="1"/>
+    <col min="20" max="20" width="24.6640625" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="str">
         <f>'Plan A - 17 Ppl'!B2</f>
         <v>PLAN A || People Count = 17</v>
@@ -627,7 +630,7 @@
       <c r="U2" s="9"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -695,7 +698,7 @@
       </c>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -763,7 +766,7 @@
       </c>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -831,7 +834,7 @@
       </c>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -899,7 +902,7 @@
       </c>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -967,7 +970,7 @@
       </c>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1035,7 +1038,7 @@
       </c>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1106,7 @@
       </c>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1174,7 @@
       </c>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1239,7 +1242,7 @@
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1275,7 +1278,7 @@
       <c r="S12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1290,7 @@
       <c r="S13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1307,17 +1310,17 @@
       <c r="S14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="str">
-        <f>'Plan A - 17 Ppl'!B15</f>
-        <v>New Person</v>
-      </c>
-      <c r="C15">
-        <f>'Plan A - 17 Ppl'!C15</f>
+    <row r="15" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f>'Plan A - 17 Ppl'!B16</f>
+        <v>New Person</v>
+      </c>
+      <c r="C15" s="1">
+        <f>'Plan A - 17 Ppl'!C16</f>
+        <v>13</v>
       </c>
       <c r="D15" s="2"/>
       <c r="G15" s="2"/>
@@ -1327,17 +1330,17 @@
       <c r="S15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="str">
-        <f>'Plan A - 17 Ppl'!B16</f>
-        <v>New Person</v>
-      </c>
-      <c r="C16" s="1">
-        <f>'Plan A - 17 Ppl'!C16</f>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>13</v>
+      </c>
+      <c r="B16" t="str">
+        <f>'Plan A - 17 Ppl'!B17</f>
+        <v>New Person</v>
+      </c>
+      <c r="C16">
+        <f>'Plan A - 17 Ppl'!C17</f>
+        <v>14</v>
       </c>
       <c r="D16" s="2"/>
       <c r="G16" s="2"/>
@@ -1347,17 +1350,17 @@
       <c r="S16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="str">
-        <f>'Plan A - 17 Ppl'!B17</f>
-        <v>New Person</v>
-      </c>
-      <c r="C17">
-        <f>'Plan A - 17 Ppl'!C17</f>
+    <row r="17" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f>'Plan A - 17 Ppl'!B18</f>
+        <v>New Person</v>
+      </c>
+      <c r="C17" s="1">
+        <f>'Plan A - 17 Ppl'!C18</f>
+        <v>15</v>
       </c>
       <c r="D17" s="2"/>
       <c r="G17" s="2"/>
@@ -1367,17 +1370,17 @@
       <c r="S17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1" t="str">
-        <f>'Plan A - 17 Ppl'!B18</f>
-        <v>New Person</v>
-      </c>
-      <c r="C18" s="1">
-        <f>'Plan A - 17 Ppl'!C18</f>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>15</v>
+      </c>
+      <c r="B18" t="str">
+        <f>'Plan A - 17 Ppl'!B19</f>
+        <v>New Person</v>
+      </c>
+      <c r="C18">
+        <f>'Plan A - 17 Ppl'!C19</f>
+        <v>16</v>
       </c>
       <c r="D18" s="2"/>
       <c r="G18" s="2"/>
@@ -1387,17 +1390,15 @@
       <c r="S18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="str">
-        <f>'Plan A - 17 Ppl'!B19</f>
-        <v>New Person</v>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
       </c>
       <c r="C19">
-        <f>'Plan A - 17 Ppl'!C19</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2"/>
       <c r="G19" s="2"/>
@@ -1407,7 +1408,7 @@
       <c r="S19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1416,8 +1417,7 @@
         <v>New Person</v>
       </c>
       <c r="C20" s="1">
-        <f>'Plan A - 17 Ppl'!C20</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D20" s="2"/>
       <c r="G20" s="2"/>
@@ -1427,12 +1427,12 @@
       <c r="S20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="22" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>'Plan A - 17 Ppl'!B23</f>
@@ -1477,7 +1477,7 @@
       <c r="U23" s="9"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2133,7 +2133,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -2145,7 +2145,7 @@
       <c r="S34" s="2"/>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="U35" s="1"/>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="S36" s="2"/>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
@@ -2229,7 +2229,7 @@
       <c r="U37" s="1"/>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="S38" s="2"/>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="U39" s="1"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="S40" s="2"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -2363,20 +2363,20 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN A || People Count = " &amp; C20</f>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2503,12 +2503,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2592,21 +2592,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="str">
         <f>"PLAN A || People Count = " &amp; C41</f>
         <v>PLAN A || People Count = 17</v>
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2725,12 +2725,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -2831,20 +2831,20 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN B || People Count = " &amp; C12</f>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2971,62 +2971,62 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>"PLAN B || People Count = " &amp; C33</f>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -3153,48 +3153,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -3218,20 +3218,20 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN C || People Count = " &amp; C12</f>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -3358,62 +3358,62 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>"PLAN C || People Count = " &amp; C33</f>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -3540,48 +3540,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -3605,20 +3605,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN D || People Count = " &amp; C11</f>
@@ -3626,7 +3626,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3733,69 +3733,69 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>"PLAN D || People Count = " &amp; C32</f>
@@ -3803,7 +3803,7 @@
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3910,55 +3910,55 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -3982,20 +3982,20 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN E || People Count = " &amp; C11</f>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4107,69 +4107,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>"PLAN E || People Count = " &amp; C32</f>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -4281,55 +4281,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -4353,20 +4353,20 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN F || People Count = " &amp; 7</f>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4477,69 +4477,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>"PLAN F || People Count = " &amp; 7</f>
@@ -4547,7 +4547,7 @@
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -4650,55 +4650,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -4722,20 +4722,20 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="str">
         <f>"PLAN G || People Count = " &amp; 6 &amp; " (Including me)"</f>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4846,69 +4846,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="str">
         <f>"PLAN G || People Count = " &amp; 6 &amp; " (Including me)"</f>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -5019,55 +5019,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>